<commit_message>
Prompt engineering part fixed
</commit_message>
<xml_diff>
--- a/data/CBM_data/Data_CBM_with_GitHub_URLs.xlsx
+++ b/data/CBM_data/Data_CBM_with_GitHub_URLs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Workspace\SCAI_code\data\CBM_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1104C8-0165-4788-9A87-8F2108F21929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{547533F2-CE60-490F-A4EC-C93A6B2DDBB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1516,7 +1516,7 @@
     <t>https://raw.githubusercontent.com/Elly0w0/image-based-information-extraction-LLM-main/main/data/CBM_data/images_CBM/image_100.jpg</t>
   </si>
   <si>
-    <t>Old_URL</t>
+    <t>GitHub_URL</t>
   </si>
 </sst>
 </file>
@@ -1892,7 +1892,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>498</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -1907,7 +1907,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1</v>
+        <v>498</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>